<commit_message>
confirmation by e-mail, creation without duplicates
</commit_message>
<xml_diff>
--- a/MovieSearch/Example.xlsx
+++ b/MovieSearch/Example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Назва</t>
   </si>
@@ -82,31 +82,13 @@
   </si>
   <si>
     <t>Рік</t>
-  </si>
-  <si>
-    <t>проол</t>
-  </si>
-  <si>
-    <t>лдд</t>
-  </si>
-  <si>
-    <t>апр</t>
-  </si>
-  <si>
-    <t>прр</t>
-  </si>
-  <si>
-    <t>пррллш</t>
-  </si>
-  <si>
-    <t>Іамзе Сухіташвілі</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +113,6 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF3E3F3A"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,11 +134,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -465,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,35 +518,6 @@
       </c>
       <c r="P2">
         <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3">
-        <v>2001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>